<commit_message>
Added sources and revised data
Added ICCT data, corrected scale of numbers. Distinguished real and forecast data
</commit_message>
<xml_diff>
--- a/figures/forecasts_literature/data/data.xlsx
+++ b/figures/forecasts_literature/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barend/Desktop/Thesis/demandmap/figures/forecasts_literature/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d6c822ed0288754/Documents/GitHub/demandmap/figures/forecasts_literature/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1350E744-A105-5E49-A92A-9524CBF4036E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:1_{1350E744-A105-5E49-A92A-9524CBF4036E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0D3FEBC-5744-4E6F-8057-FCCC74811CA5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20160" xr2:uid="{34CC2823-3E1E-5842-A042-EFB900F9BFDA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{34CC2823-3E1E-5842-A042-EFB900F9BFDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Airbus (2023)" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="ATAG (2021)" sheetId="4" r:id="rId4"/>
     <sheet name="ATI - FlyZero (2022)" sheetId="5" r:id="rId5"/>
     <sheet name=" JADC (2022)" sheetId="6" r:id="rId6"/>
-    <sheet name="Real numbers IATA" sheetId="7" r:id="rId7"/>
+    <sheet name="ICCT (2022)" sheetId="8" r:id="rId7"/>
+    <sheet name="Real numbers IATA" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="81">
   <si>
     <t>year</t>
   </si>
@@ -282,6 +283,9 @@
   </si>
   <si>
     <t>2020/06</t>
+  </si>
+  <si>
+    <t>https://theicct.org/wp-content/uploads/2022/06/Aviation-2050-Report-A4-v6.pdf</t>
   </si>
 </sst>
 </file>
@@ -289,9 +293,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.00000E+00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -348,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -361,8 +365,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -380,6 +387,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -701,18 +712,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC34834-2A60-3845-BB46-45BE6CCB4D93}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -732,12 +743,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2023</v>
       </c>
       <c r="B2" s="2">
-        <v>9686718070</v>
+        <v>9686718070000</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -752,13 +763,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2024</v>
       </c>
       <c r="B3">
         <f>B2+(B2*(D3/100))</f>
-        <v>10035439920.52</v>
+        <v>10035439920520</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -770,13 +781,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2025</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B21" si="0">B3+(B3*(D4/100))</f>
-        <v>10396715757.65872</v>
+        <v>10396715757658.721</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -788,13 +799,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>2026</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>10770997524.934435</v>
+        <v>10770997524934.436</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -806,13 +817,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2027</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>11158753435.832075</v>
+        <v>11158753435832.076</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -824,13 +835,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2028</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>11560468559.52203</v>
+        <v>11560468559522.031</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -842,13 +853,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>2029</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>11976645427.664824</v>
+        <v>11976645427664.824</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -860,13 +871,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>2030</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>12407804663.060757</v>
+        <v>12407804663060.758</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -878,13 +889,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>2031</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>12854485630.930944</v>
+        <v>12854485630930.945</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -896,13 +907,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2032</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>13317247113.644459</v>
+        <v>13317247113644.459</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -914,13 +925,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>2033</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>13796668009.735659</v>
+        <v>13796668009735.66</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -932,13 +943,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>2034</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>14293348058.086142</v>
+        <v>14293348058086.145</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -950,13 +961,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>2035</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>14807908588.177242</v>
+        <v>14807908588177.246</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -968,13 +979,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>2036</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>15340993297.351624</v>
+        <v>15340993297351.627</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -986,13 +997,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>2037</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>15893269056.056282</v>
+        <v>15893269056056.285</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -1004,13 +1015,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2038</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>16465426742.074308</v>
+        <v>16465426742074.313</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -1022,13 +1033,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2039</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>17058182104.788984</v>
+        <v>17058182104788.988</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -1040,13 +1051,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2040</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>17672276660.561386</v>
+        <v>17672276660561.391</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -1058,13 +1069,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2041</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>18308478620.341595</v>
+        <v>18308478620341.602</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -1076,13 +1087,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>2042</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>18967583850.673893</v>
+        <v>18967583850673.898</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -1109,17 +1120,17 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1139,13 +1150,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2022</v>
       </c>
       <c r="B2">
-        <f>6000*1000000</f>
-        <v>6000000000</v>
+        <f>6000*1000000000</f>
+        <v>6000000000000</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -1154,17 +1165,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2023</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>6800000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2024</v>
       </c>
       <c r="B4">
-        <v>6842105263.1999998</v>
+        <v>7600000000000</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1174,12 +1188,12 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>2025</v>
       </c>
       <c r="B5">
-        <v>7684210526.3999996</v>
+        <v>8400000000000</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -1189,12 +1203,12 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2026</v>
       </c>
       <c r="B6">
-        <v>8526315789.6000004</v>
+        <v>9200000000000</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1204,12 +1218,12 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2027</v>
       </c>
       <c r="B7">
-        <v>9368421052.7999992</v>
+        <v>10000000000000</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -1219,12 +1233,12 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>2028</v>
       </c>
       <c r="B8">
-        <v>10210526316</v>
+        <v>10800000000000</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -1234,12 +1248,12 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>2029</v>
       </c>
       <c r="B9">
-        <v>11052631579.200001</v>
+        <v>11600000000000</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -1249,12 +1263,12 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>2030</v>
       </c>
       <c r="B10">
-        <v>11894736842.400002</v>
+        <v>12400000000000</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -1264,12 +1278,12 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2031</v>
       </c>
       <c r="B11">
-        <v>12736842105.6</v>
+        <v>13200000000000</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -1279,12 +1293,12 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>2032</v>
       </c>
       <c r="B12">
-        <v>13578947368.799999</v>
+        <v>14000000000000</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -1294,12 +1308,12 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>2033</v>
       </c>
       <c r="B13">
-        <v>14421052632</v>
+        <v>14800000000000</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -1309,12 +1323,12 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>2034</v>
       </c>
       <c r="B14">
-        <v>15263157895.200001</v>
+        <v>15600000000000</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -1324,12 +1338,12 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>2035</v>
       </c>
       <c r="B15">
-        <v>16105263158.400002</v>
+        <v>16400000000000</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -1339,12 +1353,12 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>2036</v>
       </c>
       <c r="B16">
-        <v>16947368421.6</v>
+        <v>17200000000000</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -1354,12 +1368,12 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2037</v>
       </c>
       <c r="B17">
-        <v>17789473684.800003</v>
+        <v>18000000000000</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -1369,12 +1383,12 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2038</v>
       </c>
       <c r="B18">
-        <v>18631578948</v>
+        <v>18800000000000</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -1384,12 +1398,12 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2039</v>
       </c>
       <c r="B19">
-        <v>19473684211.200001</v>
+        <v>19600000000000</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -1399,12 +1413,12 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2040</v>
       </c>
       <c r="B20">
-        <v>20315789474.400002</v>
+        <v>20400000000000</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -1414,12 +1428,12 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>2041</v>
       </c>
       <c r="B21">
-        <v>21157894737.599998</v>
+        <v>21200000000000</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -1429,12 +1443,12 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>2042</v>
       </c>
       <c r="B22">
-        <v>22000000000</v>
+        <v>22000000000000</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -1454,17 +1468,17 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1484,12 +1498,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2023</v>
       </c>
       <c r="B2" s="2">
-        <v>8490000000</v>
+        <v>8490000000000</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1504,13 +1518,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2024</v>
       </c>
       <c r="B3">
         <f>$B$2+$B$2*((D3-100)/100)</f>
-        <v>8914500000</v>
+        <v>8914500000000</v>
       </c>
       <c r="D3">
         <v>105</v>
@@ -1519,13 +1533,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2025</v>
       </c>
       <c r="B4">
         <f>$B$2+$B$2*((D4-100)/100)</f>
-        <v>9381450000</v>
+        <v>9381450000000</v>
       </c>
       <c r="D4">
         <v>110.5</v>
@@ -1534,13 +1548,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>2026</v>
       </c>
       <c r="B5">
         <f t="shared" ref="B5:B9" si="0">$B$2+$B$2*((D5-100)/100)</f>
-        <v>9958770000</v>
+        <v>9958770000000</v>
       </c>
       <c r="D5">
         <v>117.3</v>
@@ -1549,13 +1563,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2027</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>10476660000</v>
+        <v>10476660000000</v>
       </c>
       <c r="D6">
         <v>123.4</v>
@@ -1564,13 +1578,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2028</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>10969080000</v>
+        <v>10969080000000</v>
       </c>
       <c r="D7">
         <v>129.19999999999999</v>
@@ -1579,13 +1593,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>2029</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>11444520000</v>
+        <v>11444520000000</v>
       </c>
       <c r="D8">
         <v>134.80000000000001</v>
@@ -1594,13 +1608,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>2030</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>11902980000</v>
+        <v>11902980000000</v>
       </c>
       <c r="D9">
         <v>140.19999999999999</v>
@@ -1609,40 +1623,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:5">
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:5">
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:5">
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:5">
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:5">
       <c r="E21" s="1"/>
     </row>
   </sheetData>
@@ -1655,17 +1669,17 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1685,12 +1699,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2019</v>
       </c>
       <c r="B2">
-        <v>8490000000</v>
+        <v>8490000000000</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -1705,13 +1719,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3">
         <f>B2+(B2*(D3/100))</f>
-        <v>8753190000</v>
+        <v>8753190000000</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1721,13 +1735,13 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2021</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B32" si="0">B3+(B3*(D4/100))</f>
-        <v>9024538890</v>
+        <v>9024538890000</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1737,13 +1751,13 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>2022</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>9304299595.5900002</v>
+        <v>9304299595590</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -1753,13 +1767,13 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2023</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>9592732883.0532894</v>
+        <v>9592732883053.2891</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1769,13 +1783,13 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>9890107602.4279423</v>
+        <v>9890107602427.9414</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -1785,13 +1799,13 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>10196700938.103209</v>
+        <v>10196700938103.207</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -1801,13 +1815,13 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>2026</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>10512798667.184408</v>
+        <v>10512798667184.406</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -1817,13 +1831,13 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>2027</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>10838695425.867125</v>
+        <v>10838695425867.123</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -1833,13 +1847,13 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2028</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>11174694984.069006</v>
+        <v>11174694984069.004</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -1849,13 +1863,13 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>2029</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>11521110528.575146</v>
+        <v>11521110528575.143</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -1865,13 +1879,13 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>2030</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>11878264954.960976</v>
+        <v>11878264954960.973</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -1881,13 +1895,13 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>2031</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>12246491168.564766</v>
+        <v>12246491168564.764</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -1897,13 +1911,13 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>2032</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>12626132394.790274</v>
+        <v>12626132394790.271</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -1913,13 +1927,13 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>2033</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>13017542499.028772</v>
+        <v>13017542499028.77</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -1929,13 +1943,13 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2034</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>13421086316.498665</v>
+        <v>13421086316498.662</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -1945,13 +1959,13 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2035</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>13837139992.310123</v>
+        <v>13837139992310.121</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -1961,13 +1975,13 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2036</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>14266091332.071737</v>
+        <v>14266091332071.734</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -1977,13 +1991,13 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2037</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>14708340163.365961</v>
+        <v>14708340163365.959</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -1993,13 +2007,13 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>2038</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>15164298708.430305</v>
+        <v>15164298708430.305</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -2009,13 +2023,13 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>2039</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>15634391968.391645</v>
+        <v>15634391968391.645</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -2024,13 +2038,13 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>2040</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>16119058119.411787</v>
+        <v>16119058119411.785</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -2039,13 +2053,13 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>2041</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>16618748921.113552</v>
+        <v>16618748921113.551</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -2054,13 +2068,13 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>2042</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>17133930137.668072</v>
+        <v>17133930137668.07</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -2069,13 +2083,13 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>2043</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>17665081971.935783</v>
+        <v>17665081971935.781</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -2084,13 +2098,13 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>2044</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>18212699513.065792</v>
+        <v>18212699513065.789</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -2099,13 +2113,13 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>2045</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>18777293197.970833</v>
+        <v>18777293197970.828</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -2114,13 +2128,13 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>2046</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>19359389287.107929</v>
+        <v>19359389287107.922</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -2129,13 +2143,13 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>2047</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>19959530355.008274</v>
+        <v>19959530355008.266</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -2144,13 +2158,13 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>2048</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>20578275796.013531</v>
+        <v>20578275796013.523</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -2159,13 +2173,13 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>2049</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>21216202345.689949</v>
+        <v>21216202345689.941</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -2174,12 +2188,12 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>2050</v>
       </c>
       <c r="B33">
-        <v>22000000000</v>
+        <v>22000000000000</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -2201,17 +2215,17 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2231,12 +2245,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2019</v>
       </c>
       <c r="B2">
-        <v>8540000000</v>
+        <v>8540000000000</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -2251,13 +2265,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3">
         <f>B2+(B2*(D3/100))</f>
-        <v>8813280000</v>
+        <v>8813280000000</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -2267,13 +2281,13 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2021</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B32" si="0">B3+(B3*(D4/100))</f>
-        <v>9095304960</v>
+        <v>9095304960000</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -2283,13 +2297,13 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>2022</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>9386354718.7199993</v>
+        <v>9386354718720</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -2299,13 +2313,13 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2023</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>9686718069.7190399</v>
+        <v>9686718069719.0391</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -2315,13 +2329,13 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>9996693047.9500484</v>
+        <v>9996693047950.0488</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -2331,12 +2345,12 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8">
-        <v>10830000000</v>
+        <v>10830000000000</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -2346,13 +2360,13 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>2026</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>11176560000</v>
+        <v>11176560000000</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -2362,13 +2376,13 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>2027</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>11534209920</v>
+        <v>11534209920000</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2378,13 +2392,13 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2028</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>11903304637.440001</v>
+        <v>11903304637440</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -2394,13 +2408,13 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>2029</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>12284210385.838081</v>
+        <v>12284210385838.08</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2410,12 +2424,12 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>2030</v>
       </c>
       <c r="B13">
-        <v>13120000000</v>
+        <v>13120000000000</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
@@ -2425,13 +2439,13 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>2031</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>13539840000</v>
+        <v>13539840000000</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -2441,13 +2455,13 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>2032</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>13973114880</v>
+        <v>13973114880000</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -2457,13 +2471,13 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>2033</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>14420254556.16</v>
+        <v>14420254556160</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -2473,13 +2487,13 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2034</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>14881702701.957119</v>
+        <v>14881702701957.119</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -2489,13 +2503,13 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2035</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>15357917188.419746</v>
+        <v>15357917188419.746</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -2505,13 +2519,13 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2036</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>15849370538.449179</v>
+        <v>15849370538449.178</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -2521,13 +2535,13 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2037</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>16356550395.679552</v>
+        <v>16356550395679.551</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -2537,13 +2551,13 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>2038</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>16879960008.341297</v>
+        <v>16879960008341.297</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -2553,13 +2567,13 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>2039</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>17420118728.608219</v>
+        <v>17420118728608.219</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -2568,12 +2582,12 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>2040</v>
       </c>
       <c r="B23">
-        <v>17860000000</v>
+        <v>17860000000000</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -2582,13 +2596,13 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>2041</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>18431520000</v>
+        <v>18431520000000</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -2597,13 +2611,13 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>2042</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>19021328640</v>
+        <v>19021328640000</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -2612,13 +2626,13 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>2043</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>19630011156.48</v>
+        <v>19630011156480</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -2627,13 +2641,13 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>2044</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>20258171513.487358</v>
+        <v>20258171513487.359</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -2642,13 +2656,13 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>2045</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>20906433001.918953</v>
+        <v>20906433001918.953</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -2657,13 +2671,13 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>2046</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>21575438857.980358</v>
+        <v>21575438857980.359</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -2672,13 +2686,13 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>2047</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>22265852901.43573</v>
+        <v>22265852901435.73</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -2687,13 +2701,13 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>2048</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>22978360194.281673</v>
+        <v>22978360194281.672</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -2702,13 +2716,13 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>2049</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>23713667720.498688</v>
+        <v>23713667720498.684</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -2717,12 +2731,12 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>2050</v>
       </c>
       <c r="B33">
-        <v>22880000000</v>
+        <v>22880000000000</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>12</v>
@@ -2748,17 +2762,17 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.625" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2778,12 +2792,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2019</v>
       </c>
       <c r="B2">
-        <v>8486000000</v>
+        <v>8486000000000</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -2798,13 +2812,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3">
         <f>B2+(B2*(D3/100))</f>
-        <v>8775372600</v>
+        <v>8775372600000</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -2814,13 +2828,13 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2021</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B24" si="0">B3+(B3*(D4/100))</f>
-        <v>9074612805.6599998</v>
+        <v>9074612805660</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -2830,13 +2844,13 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>2022</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>9384057102.3330059</v>
+        <v>9384057102333.0059</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -2846,13 +2860,13 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2023</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>9704053449.522562</v>
+        <v>9704053449522.5605</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -2862,13 +2876,13 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>10034961672.151281</v>
+        <v>10034961672151.279</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -2878,13 +2892,13 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>10377153865.17164</v>
+        <v>10377153865171.639</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -2894,13 +2908,13 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>2026</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>10731014811.973993</v>
+        <v>10731014811973.992</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -2910,13 +2924,13 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>2027</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>11096942417.062307</v>
+        <v>11096942417062.305</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2926,13 +2940,13 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2028</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>11475348153.484133</v>
+        <v>11475348153484.129</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -2942,13 +2956,13 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>2029</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>11866657525.517942</v>
+        <v>11866657525517.938</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2958,13 +2972,13 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>2030</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>12271310547.138103</v>
+        <v>12271310547138.1</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -2974,13 +2988,13 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>2031</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>12689762236.795513</v>
+        <v>12689762236795.508</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -2990,13 +3004,13 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>2032</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>13122483129.07024</v>
+        <v>13122483129070.234</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -3006,13 +3020,13 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>2033</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>13569959803.771536</v>
+        <v>13569959803771.529</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -3022,13 +3036,13 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2034</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>14032695433.080145</v>
+        <v>14032695433080.139</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -3038,13 +3052,13 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2035</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>14511210347.348177</v>
+        <v>14511210347348.172</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -3054,13 +3068,13 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2036</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>15006042620.192749</v>
+        <v>15006042620192.744</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -3070,13 +3084,13 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2037</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>15517748673.541321</v>
+        <v>15517748673541.316</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -3086,13 +3100,13 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>2038</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>16046903903.30908</v>
+        <v>16046903903309.076</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -3102,13 +3116,13 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>2039</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>16594103326.411921</v>
+        <v>16594103326411.916</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -3117,13 +3131,13 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>2040</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>17159962249.842567</v>
+        <v>17159962249842.563</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -3132,13 +3146,13 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>2041</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>17745116962.562199</v>
+        <v>17745116962562.195</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -3156,21 +3170,342 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EB8B21-702D-7B44-9AAA-37E8D9323EE6}">
-  <dimension ref="A1:D67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1904D647-5F83-4FE8-AD27-60F731A40BD2}">
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView zoomScale="143" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.5" customWidth="1"/>
+    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3">
+        <v>2500000000000</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>2021</v>
+      </c>
+      <c r="B4">
+        <v>4000000000000</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5">
+        <v>5500000000000</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>2023</v>
+      </c>
+      <c r="B6">
+        <v>7000000000000</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>2024</v>
+      </c>
+      <c r="B7">
+        <v>8500000000000</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8">
+        <v>10000000000000</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>2026</v>
+      </c>
+      <c r="B9">
+        <v>10400000000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>2027</v>
+      </c>
+      <c r="B10">
+        <v>10800000000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>2028</v>
+      </c>
+      <c r="B11">
+        <v>11200000000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>2029</v>
+      </c>
+      <c r="B12">
+        <v>11600000000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>2030</v>
+      </c>
+      <c r="B13">
+        <v>12000000000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>2031</v>
+      </c>
+      <c r="B14">
+        <v>12400000000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>2032</v>
+      </c>
+      <c r="B15">
+        <v>12800000000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>2033</v>
+      </c>
+      <c r="B16">
+        <v>13200000000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>2034</v>
+      </c>
+      <c r="B17">
+        <v>13600000000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>2035</v>
+      </c>
+      <c r="B18">
+        <v>14000000000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>2036</v>
+      </c>
+      <c r="B19">
+        <v>14400000000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>2037</v>
+      </c>
+      <c r="B20">
+        <v>14800000000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>2038</v>
+      </c>
+      <c r="B21">
+        <v>15200000000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>2039</v>
+      </c>
+      <c r="B22">
+        <v>15600000000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>2040</v>
+      </c>
+      <c r="B23">
+        <v>16000000000000</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>2041</v>
+      </c>
+      <c r="B24">
+        <v>16600000000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>2042</v>
+      </c>
+      <c r="B25">
+        <v>17200000000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>2043</v>
+      </c>
+      <c r="B26">
+        <v>17800000000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>2044</v>
+      </c>
+      <c r="B27">
+        <v>18400000000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>2045</v>
+      </c>
+      <c r="B28">
+        <v>19000000000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>2046</v>
+      </c>
+      <c r="B29">
+        <v>19600000000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>2047</v>
+      </c>
+      <c r="B30">
+        <v>20200000000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>2048</v>
+      </c>
+      <c r="B31">
+        <v>20800000000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>2049</v>
+      </c>
+      <c r="B32">
+        <v>21400000000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>2050</v>
+      </c>
+      <c r="B33">
+        <v>22000000000000</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{308EE87A-7AA4-4712-81F8-D9671B681E5F}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{6BDD0C01-DCEB-409A-B549-57AFA1CDAE69}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EB8B21-702D-7B44-9AAA-37E8D9323EE6}">
+  <dimension ref="A1:F67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="143" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.375" customWidth="1"/>
+    <col min="5" max="6" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
@@ -3178,790 +3513,1140 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
-        <f>D2/100</f>
+      <c r="B2" s="3">
+        <f>E2*10</f>
+        <v>6379310344827.5801</v>
+      </c>
+      <c r="C2">
+        <f>E2/100</f>
         <v>6379310344.8275805</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>637931034482.75806</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F2" s="7">
+        <f>SUM(E2:E11)</f>
+        <v>6977931034482.7549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3">
-        <f>D3/100</f>
+      <c r="B3" s="3">
+        <f t="shared" ref="B3:B66" si="0">E3*10</f>
+        <v>5993103448275.8604</v>
+      </c>
+      <c r="C3">
+        <f>E3/100</f>
         <v>5993103448.2758608</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>599310344827.58606</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4">
-        <f t="shared" ref="B4:B66" si="0">D4/100</f>
+      <c r="B4" s="3">
+        <f t="shared" si="0"/>
+        <v>6806896551724.1299</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C66" si="1">E4/100</f>
         <v>6806896551.7241297</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>680689655172.41296</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
+      <c r="B5" s="3">
+        <f t="shared" si="0"/>
+        <v>6779310344827.5801</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
         <v>6779310344.8275805</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>677931034482.75806</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>7262068965517.2402</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
         <v>7262068965.5172396</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>726206896551.724</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>7965517241379.3105</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
         <v>7965517241.3793106</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>796551724137.93103</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>7937931034482.75</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
         <v>7937931034.4827499</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>793793103448.27502</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>7055172413793.1006</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
         <v>7055172413.7931004</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>705517241379.31006</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>7096551724137.9297</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
         <v>7096551724.1379299</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>709655172413.79297</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>6503448275862.0605</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
         <v>6503448275.8620605</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>650344827586.20605</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>6268965517241.3789</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
         <v>6268965517.2413797</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>626896551724.13794</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F12" s="7">
+        <f>SUM(E12:E21)</f>
+        <v>7291034482758.6182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>7041379310344.8203</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
         <v>7041379310.344821</v>
       </c>
-      <c r="D13" s="6">
+      <c r="E13" s="6">
         <v>704137931034.48206</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>7068965517241.3789</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
         <v>7068965517.2413797</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <v>706896551724.13794</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>7193103448275.8604</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
         <v>7193103448.2758608</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <v>719310344827.58606</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>7579310344827.5801</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
         <v>7579310344.8275805</v>
       </c>
-      <c r="D16" s="3">
+      <c r="E16" s="3">
         <v>757931034482.75806</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
+      <c r="B17" s="3">
+        <f t="shared" si="0"/>
+        <v>8200000000000</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
         <v>8200000000</v>
       </c>
-      <c r="D17" s="3">
+      <c r="E17" s="3">
         <v>820000000000</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
+      <c r="B18" s="3">
+        <f t="shared" si="0"/>
+        <v>8213793103448.2705</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
         <v>8213793103.4482698</v>
       </c>
-      <c r="D18" s="3">
+      <c r="E18" s="3">
         <v>821379310344.82703</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>7303448275862.0605</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
         <v>7303448275.8620605</v>
       </c>
-      <c r="D19" s="3">
+      <c r="E19" s="3">
         <v>730344827586.20605</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>7317241379310.3408</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
         <v>7317241379.3103409</v>
       </c>
-      <c r="D20" s="3">
+      <c r="E20" s="3">
         <v>731724137931.03406</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
+      <c r="B21" s="3">
+        <f t="shared" si="0"/>
+        <v>6724137931034.4805</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
         <v>6724137931.0344801</v>
       </c>
-      <c r="D21" s="3">
+      <c r="E21" s="3">
         <v>672413793103.448</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>7137931034482.75</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
         <v>7137931034.4827499</v>
       </c>
-      <c r="D22" s="3">
+      <c r="E22" s="3">
         <v>713793103448.27502</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F22" s="7">
+        <f>SUM(E22:E32)</f>
+        <v>3211034482750.5479</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
+      <c r="B23" s="3">
+        <f t="shared" si="0"/>
+        <v>6958620689655.1699</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
         <v>6958620689.6551695</v>
       </c>
-      <c r="D23" s="3">
+      <c r="E23" s="3">
         <v>695862068965.51697</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
+      <c r="B24" s="3">
+        <f t="shared" si="0"/>
+        <v>4482758620608.96</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
         <v>4482758620.6089602</v>
       </c>
-      <c r="D24" s="3">
+      <c r="E24" s="3">
         <v>448275862060.896</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
+      <c r="B25" s="3">
+        <f t="shared" si="0"/>
+        <v>2034482758620.6899</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
         <v>2034482758.6206901</v>
       </c>
-      <c r="D25" s="3">
+      <c r="E25" s="3">
         <v>203448275862.069</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
+      <c r="B26" s="3">
+        <f t="shared" si="0"/>
+        <v>448275862068.96698</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
         <v>448275862.06896698</v>
       </c>
-      <c r="D26" s="3">
+      <c r="E26" s="3">
         <v>44827586206.896698</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
+      <c r="B27" s="3">
+        <f t="shared" si="0"/>
+        <v>1041379310344.8199</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
         <v>1041379310.3448199</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>104137931034.48199</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
+      <c r="B28" s="3">
+        <f t="shared" si="0"/>
+        <v>1717241379310.3398</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
         <v>1717241379.3103399</v>
       </c>
-      <c r="D28" s="3">
+      <c r="E28" s="3">
         <v>171724137931.034</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
+      <c r="B29" s="3">
+        <f t="shared" si="0"/>
+        <v>2089655172413.79</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
         <v>2089655172.41379</v>
       </c>
-      <c r="D29" s="3">
+      <c r="E29" s="3">
         <v>208965517241.379</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
+      <c r="B30" s="3">
+        <f t="shared" si="0"/>
+        <v>2048275862068.96</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
         <v>2048275862.06896</v>
       </c>
-      <c r="D30" s="3">
+      <c r="E30" s="3">
         <v>204827586206.896</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
+      <c r="B31" s="3">
+        <f t="shared" si="0"/>
+        <v>2158620689655.1699</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
         <v>2158620689.65517</v>
       </c>
-      <c r="D31" s="3">
+      <c r="E31" s="3">
         <v>215862068965.517</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
+      <c r="B32" s="3">
+        <f t="shared" si="0"/>
+        <v>1993103448275.8599</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
         <v>1993103448.2758601</v>
       </c>
-      <c r="D32" s="3">
+      <c r="E32" s="3">
         <v>199310344827.586</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B33">
-        <f t="shared" si="0"/>
+      <c r="B33" s="3">
+        <f t="shared" si="0"/>
+        <v>2186206896551.72</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
         <v>2186206896.5517201</v>
       </c>
-      <c r="D33" s="3">
+      <c r="E33" s="3">
         <v>218620689655.172</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F33" s="7">
+        <f>SUM(E33:E41)</f>
+        <v>2628275862068.9609</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
+      <c r="B34" s="3">
+        <f t="shared" si="0"/>
+        <v>1606896551724.1299</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
         <v>1606896551.7241299</v>
       </c>
-      <c r="D34" s="3">
+      <c r="E34" s="3">
         <v>160689655172.41299</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
+      <c r="B35" s="3">
+        <f t="shared" si="0"/>
+        <v>2351724137931.0298</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
         <v>2351724137.9310298</v>
       </c>
-      <c r="D35" s="3">
+      <c r="E35" s="3">
         <v>235172413793.103</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B36">
-        <f t="shared" si="0"/>
+      <c r="B36" s="3">
+        <f t="shared" si="0"/>
+        <v>2475862068965.5098</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
         <v>2475862068.9655099</v>
       </c>
-      <c r="D36" s="3">
+      <c r="E36" s="3">
         <v>247586206896.55099</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B37">
-        <f t="shared" si="0"/>
+      <c r="B37" s="3">
+        <f t="shared" si="0"/>
+        <v>3055172413793.1001</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
         <v>3055172413.7930999</v>
       </c>
-      <c r="D37" s="3">
+      <c r="E37" s="3">
         <v>305517241379.31</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B38">
-        <f t="shared" si="0"/>
+      <c r="B38" s="3">
+        <f t="shared" si="0"/>
+        <v>3827586206896.5503</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
         <v>3827586206.8965502</v>
       </c>
-      <c r="D38" s="3">
+      <c r="E38" s="3">
         <v>382758620689.65503</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B39">
-        <f t="shared" si="0"/>
+      <c r="B39" s="3">
+        <f t="shared" si="0"/>
+        <v>3455172413793.1001</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
         <v>3455172413.7930999</v>
       </c>
-      <c r="D39" s="3">
+      <c r="E39" s="3">
         <v>345517241379.31</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B40">
-        <f t="shared" si="0"/>
+      <c r="B40" s="3">
+        <f t="shared" si="0"/>
+        <v>3744827586206.8901</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
         <v>3744827586.2068901</v>
       </c>
-      <c r="D40" s="3">
+      <c r="E40" s="3">
         <v>374482758620.68903</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B41">
-        <f t="shared" si="0"/>
+      <c r="B41" s="3">
+        <f t="shared" si="0"/>
+        <v>3579310344827.5801</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
         <v>3579310344.82758</v>
       </c>
-      <c r="D41" s="3">
+      <c r="E41" s="3">
         <v>357931034482.758</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B42">
-        <f t="shared" si="0"/>
+      <c r="B42" s="3">
+        <f t="shared" si="0"/>
+        <v>3896551724137.9302</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
         <v>3896551724.1379304</v>
       </c>
-      <c r="D42" s="3">
+      <c r="E42" s="3">
         <v>389655172413.79303</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F42" s="7">
+        <f>SUM(E42:E53)</f>
+        <v>5799999999999.9961</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B43">
-        <f t="shared" si="0"/>
+      <c r="B43" s="3">
+        <f t="shared" si="0"/>
+        <v>3441379310344.8198</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
         <v>3441379310.34482</v>
       </c>
-      <c r="D43" s="3">
+      <c r="E43" s="3">
         <v>344137931034.48199</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B44">
-        <f t="shared" si="0"/>
+      <c r="B44" s="3">
+        <f t="shared" si="0"/>
+        <v>3413793103448.2705</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
         <v>3413793103.4482703</v>
       </c>
-      <c r="D44" s="3">
+      <c r="E44" s="3">
         <v>341379310344.82703</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B45">
-        <f t="shared" si="0"/>
+      <c r="B45" s="3">
+        <f t="shared" si="0"/>
+        <v>4048275862068.96</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
         <v>4048275862.0689602</v>
       </c>
-      <c r="D45" s="3">
+      <c r="E45" s="3">
         <v>404827586206.896</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B46">
-        <f t="shared" si="0"/>
+      <c r="B46" s="3">
+        <f t="shared" si="0"/>
+        <v>4365517241379.3105</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
         <v>4365517241.3793106</v>
       </c>
-      <c r="D46" s="3">
+      <c r="E46" s="3">
         <v>436551724137.93103</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B47">
-        <f t="shared" si="0"/>
+      <c r="B47" s="3">
+        <f t="shared" si="0"/>
+        <v>4944827586206.8906</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
         <v>4944827586.2068901</v>
       </c>
-      <c r="D47" s="3">
+      <c r="E47" s="3">
         <v>494482758620.68903</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B48">
-        <f t="shared" si="0"/>
+      <c r="B48" s="3">
+        <f t="shared" si="0"/>
+        <v>5468965517241.3799</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
         <v>5468965517.2413797</v>
       </c>
-      <c r="D48" s="3">
+      <c r="E48" s="3">
         <v>546896551724.138</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B49">
-        <f t="shared" si="0"/>
+      <c r="B49" s="3">
+        <f t="shared" si="0"/>
+        <v>6200000000000</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="1"/>
         <v>6200000000</v>
       </c>
-      <c r="D49" s="3">
+      <c r="E49" s="3">
         <v>620000000000</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B50">
-        <f t="shared" si="0"/>
+      <c r="B50" s="3">
+        <f t="shared" si="0"/>
+        <v>6117241379310.3408</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="1"/>
         <v>6117241379.3103409</v>
       </c>
-      <c r="D50" s="3">
+      <c r="E50" s="3">
         <v>611724137931.03406</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B51">
-        <f t="shared" si="0"/>
+      <c r="B51" s="3">
+        <f t="shared" si="0"/>
+        <v>5468965517241.3799</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="1"/>
         <v>5468965517.2413797</v>
       </c>
-      <c r="D51" s="3">
+      <c r="E51" s="3">
         <v>546896551724.138</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B52">
-        <f t="shared" si="0"/>
+      <c r="B52" s="3">
+        <f t="shared" si="0"/>
+        <v>5482758620689.6504</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="1"/>
         <v>5482758620.6896505</v>
       </c>
-      <c r="D52" s="3">
+      <c r="E52" s="3">
         <v>548275862068.96503</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B53">
-        <f t="shared" si="0"/>
+      <c r="B53" s="3">
+        <f t="shared" si="0"/>
+        <v>5151724137931.0303</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="1"/>
         <v>5151724137.9310303</v>
       </c>
-      <c r="D53" s="3">
+      <c r="E53" s="3">
         <v>515172413793.10303</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B54">
-        <f t="shared" si="0"/>
+      <c r="B54" s="3">
+        <f t="shared" si="0"/>
+        <v>5565517241379.3105</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="1"/>
         <v>5565517241.3793106</v>
       </c>
-      <c r="D54" s="3">
+      <c r="E54" s="3">
         <v>556551724137.93103</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F54" s="7">
+        <f>SUM(E54:E65)</f>
+        <v>8037241379310.3428</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B55">
-        <f t="shared" si="0"/>
+      <c r="B55" s="3">
+        <f t="shared" si="0"/>
+        <v>5800000000000</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="1"/>
         <v>5800000000</v>
       </c>
-      <c r="D55" s="3">
+      <c r="E55" s="3">
         <v>580000000000</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F55" s="7"/>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B56">
-        <f t="shared" si="0"/>
+      <c r="B56" s="3">
+        <f t="shared" si="0"/>
+        <v>5468965517241.3799</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="1"/>
         <v>5468965517.2413797</v>
       </c>
-      <c r="D56" s="3">
+      <c r="E56" s="3">
         <v>546896551724.138</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F56" s="7"/>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B57">
-        <f t="shared" si="0"/>
+      <c r="B57" s="3">
+        <f t="shared" si="0"/>
+        <v>6255172413793.1006</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="1"/>
         <v>6255172413.7931004</v>
       </c>
-      <c r="D57" s="3">
+      <c r="E57" s="3">
         <v>625517241379.31006</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B58">
-        <f t="shared" si="0"/>
+      <c r="B58" s="3">
+        <f t="shared" si="0"/>
+        <v>6420689655172.4102</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="1"/>
         <v>6420689655.17241</v>
       </c>
-      <c r="D58" s="3">
+      <c r="E58" s="3">
         <v>642068965517.24097</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B59">
-        <f t="shared" si="0"/>
+      <c r="B59" s="3">
+        <f t="shared" si="0"/>
+        <v>6944827586206.8896</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="1"/>
         <v>6944827586.2068901</v>
       </c>
-      <c r="D59" s="3">
+      <c r="E59" s="3">
         <v>694482758620.68896</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F59" s="7"/>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B60">
-        <f t="shared" si="0"/>
+      <c r="B60" s="3">
+        <f t="shared" si="0"/>
+        <v>7206896551724.1299</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="1"/>
         <v>7206896551.7241297</v>
       </c>
-      <c r="D60" s="3">
+      <c r="E60" s="3">
         <v>720689655172.41296</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B61">
-        <f t="shared" si="0"/>
+      <c r="B61" s="3">
+        <f t="shared" si="0"/>
+        <v>7896551724137.9297</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="1"/>
         <v>7896551724.1379299</v>
       </c>
-      <c r="D61" s="3">
+      <c r="E61" s="3">
         <v>789655172413.79297</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B62">
-        <f t="shared" si="0"/>
+      <c r="B62" s="3">
+        <f t="shared" si="0"/>
+        <v>7855172413793.1006</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="1"/>
         <v>7855172413.7931004</v>
       </c>
-      <c r="D62" s="3">
+      <c r="E62" s="3">
         <v>785517241379.31006</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B63">
-        <f t="shared" si="0"/>
+      <c r="B63" s="3">
+        <f t="shared" si="0"/>
+        <v>7124137931034.4805</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="1"/>
         <v>7124137931.0344801</v>
       </c>
-      <c r="D63" s="3">
+      <c r="E63" s="3">
         <v>712413793103.448</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B64">
-        <f t="shared" si="0"/>
+      <c r="B64" s="3">
+        <f t="shared" si="0"/>
+        <v>7193103448275.8604</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="1"/>
         <v>7193103448.2758608</v>
       </c>
-      <c r="D64" s="3">
+      <c r="E64" s="3">
         <v>719310344827.58606</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B65">
-        <f t="shared" si="0"/>
+      <c r="B65" s="3">
+        <f t="shared" si="0"/>
+        <v>6641379310344.8203</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="1"/>
         <v>6641379310.344821</v>
       </c>
-      <c r="D65" s="3">
+      <c r="E65" s="3">
         <v>664137931034.48206</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F65" s="7"/>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B66">
-        <f t="shared" si="0"/>
+      <c r="B66" s="3">
+        <f t="shared" si="0"/>
+        <v>6986206896551.7197</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="1"/>
         <v>6986206896.5517197</v>
       </c>
-      <c r="D66" s="3">
+      <c r="E66" s="3">
         <v>698620689655.172</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6">
       <c r="A67" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F42:F53"/>
+    <mergeCell ref="F54:F65"/>
+    <mergeCell ref="F2:F11"/>
+    <mergeCell ref="F12:F21"/>
+    <mergeCell ref="F33:F41"/>
+    <mergeCell ref="F22:F32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started with new script for world map based on eurostat API
</commit_message>
<xml_diff>
--- a/figures/forecasts_literature/data/data.xlsx
+++ b/figures/forecasts_literature/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d6c822ed0288754/Documents/GitHub/demandmap/figures/forecasts_literature/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barend/Desktop/Thesis/demandmap/figures/forecasts_literature/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{1350E744-A105-5E49-A92A-9524CBF4036E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E19C5DC3-BE07-41CF-BCD2-F2120C3667EC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29792BA-BF52-DF4E-BDB7-699FF91B9E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{34CC2823-3E1E-5842-A042-EFB900F9BFDA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20160" firstSheet="1" activeTab="8" xr2:uid="{34CC2823-3E1E-5842-A042-EFB900F9BFDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Airbus (2023)" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,11 @@
     <sheet name="Bain &amp; Company (2023)" sheetId="3" r:id="rId3"/>
     <sheet name="ATAG (2021)" sheetId="4" r:id="rId4"/>
     <sheet name="ATI - FlyZero (2022)" sheetId="5" r:id="rId5"/>
-    <sheet name=" JADC (2022)" sheetId="6" r:id="rId6"/>
+    <sheet name="JADC (2022)" sheetId="6" r:id="rId6"/>
     <sheet name="ICCT (2022)" sheetId="8" r:id="rId7"/>
     <sheet name="Real numbers IATA" sheetId="7" r:id="rId8"/>
+    <sheet name="GDP upper" sheetId="9" r:id="rId9"/>
+    <sheet name="GDP lower" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="83">
   <si>
     <t>year</t>
   </si>
@@ -286,6 +288,12 @@
   </si>
   <si>
     <t>https://theicct.org/wp-content/uploads/2022/06/Aviation-2050-Report-A4-v6.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP </t>
+  </si>
+  <si>
+    <t>https://tntcat.iiasa.ac.at/SspDb/dsd?Action=htmlpage&amp;page=30</t>
   </si>
 </sst>
 </file>
@@ -295,7 +303,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000E+00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -387,10 +395,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -716,14 +720,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -743,7 +747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -763,7 +767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -781,7 +785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -799,7 +803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -817,7 +821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2027</v>
       </c>
@@ -835,7 +839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2028</v>
       </c>
@@ -853,7 +857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2029</v>
       </c>
@@ -871,7 +875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -889,7 +893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2031</v>
       </c>
@@ -907,7 +911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2032</v>
       </c>
@@ -925,7 +929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2033</v>
       </c>
@@ -943,7 +947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2034</v>
       </c>
@@ -961,7 +965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2035</v>
       </c>
@@ -979,7 +983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2036</v>
       </c>
@@ -997,7 +1001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2037</v>
       </c>
@@ -1015,13 +1019,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2038</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>16465426742074.313</v>
+        <v>16465426742074.312</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -1033,7 +1037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2039</v>
       </c>
@@ -1051,7 +1055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2040</v>
       </c>
@@ -1069,7 +1073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2041</v>
       </c>
@@ -1087,7 +1091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2042</v>
       </c>
@@ -1112,6 +1116,29 @@
     <hyperlink ref="E4:E21" r:id="rId3" display="https://www.airbus.com/en/products-services/commercial-aircraft/market/global-market-forecast " xr:uid="{A7BBD0EA-16C2-FA40-A005-AF67CCABE998}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC22BD34-57F9-594D-9269-D8E7AAAE2F1C}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1123,14 +1150,14 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +1177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2022</v>
       </c>
@@ -1165,7 +1192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2023</v>
       </c>
@@ -1173,7 +1200,7 @@
         <v>6800000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2024</v>
       </c>
@@ -1188,7 +1215,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2025</v>
       </c>
@@ -1203,7 +1230,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2026</v>
       </c>
@@ -1218,7 +1245,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2027</v>
       </c>
@@ -1233,7 +1260,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2028</v>
       </c>
@@ -1248,7 +1275,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2029</v>
       </c>
@@ -1263,7 +1290,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2030</v>
       </c>
@@ -1278,7 +1305,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2031</v>
       </c>
@@ -1293,7 +1320,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2032</v>
       </c>
@@ -1308,7 +1335,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2033</v>
       </c>
@@ -1323,7 +1350,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2034</v>
       </c>
@@ -1338,7 +1365,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2035</v>
       </c>
@@ -1353,7 +1380,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2036</v>
       </c>
@@ -1368,7 +1395,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2037</v>
       </c>
@@ -1383,7 +1410,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2038</v>
       </c>
@@ -1398,7 +1425,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2039</v>
       </c>
@@ -1413,7 +1440,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2040</v>
       </c>
@@ -1428,7 +1455,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2041</v>
       </c>
@@ -1443,7 +1470,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2042</v>
       </c>
@@ -1471,14 +1498,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1498,7 +1525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -1518,7 +1545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -1533,7 +1560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -1548,7 +1575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -1563,7 +1590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2027</v>
       </c>
@@ -1578,7 +1605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2028</v>
       </c>
@@ -1593,7 +1620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2029</v>
       </c>
@@ -1608,7 +1635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -1623,40 +1650,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="5:5">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="5:5">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="5:5">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="5:5">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="5:5">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E21" s="1"/>
     </row>
   </sheetData>
@@ -1672,14 +1699,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1699,7 +1726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -1719,7 +1746,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -1735,7 +1762,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -1751,7 +1778,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -1767,7 +1794,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -1783,7 +1810,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2024</v>
       </c>
@@ -1799,7 +1826,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2025</v>
       </c>
@@ -1815,7 +1842,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2026</v>
       </c>
@@ -1831,7 +1858,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2027</v>
       </c>
@@ -1847,7 +1874,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2028</v>
       </c>
@@ -1863,7 +1890,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2029</v>
       </c>
@@ -1879,7 +1906,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2030</v>
       </c>
@@ -1895,7 +1922,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2031</v>
       </c>
@@ -1911,7 +1938,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2032</v>
       </c>
@@ -1927,7 +1954,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2033</v>
       </c>
@@ -1943,7 +1970,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2034</v>
       </c>
@@ -1959,7 +1986,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2035</v>
       </c>
@@ -1975,7 +2002,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2036</v>
       </c>
@@ -1991,7 +2018,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2037</v>
       </c>
@@ -2007,7 +2034,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2038</v>
       </c>
@@ -2023,7 +2050,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2039</v>
       </c>
@@ -2038,7 +2065,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2040</v>
       </c>
@@ -2053,7 +2080,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2041</v>
       </c>
@@ -2068,7 +2095,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2042</v>
       </c>
@@ -2083,7 +2110,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2043</v>
       </c>
@@ -2098,7 +2125,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2044</v>
       </c>
@@ -2113,7 +2140,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2045</v>
       </c>
@@ -2128,7 +2155,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2046</v>
       </c>
@@ -2143,7 +2170,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2047</v>
       </c>
@@ -2158,7 +2185,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2048</v>
       </c>
@@ -2173,7 +2200,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2049</v>
       </c>
@@ -2188,7 +2215,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2050</v>
       </c>
@@ -2214,18 +2241,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19E5338-4817-434F-919B-9F5BFD0B85EA}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B32" sqref="B32:B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2245,7 +2272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -2265,7 +2292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -2281,7 +2308,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -2297,7 +2324,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -2313,7 +2340,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -2329,7 +2356,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2024</v>
       </c>
@@ -2345,7 +2372,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2025</v>
       </c>
@@ -2360,7 +2387,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2026</v>
       </c>
@@ -2376,7 +2403,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2027</v>
       </c>
@@ -2392,7 +2419,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2028</v>
       </c>
@@ -2408,7 +2435,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2029</v>
       </c>
@@ -2424,7 +2451,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2030</v>
       </c>
@@ -2439,7 +2466,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2031</v>
       </c>
@@ -2455,7 +2482,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2032</v>
       </c>
@@ -2471,7 +2498,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2033</v>
       </c>
@@ -2487,7 +2514,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2034</v>
       </c>
@@ -2503,7 +2530,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2035</v>
       </c>
@@ -2519,7 +2546,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2036</v>
       </c>
@@ -2535,7 +2562,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2037</v>
       </c>
@@ -2551,7 +2578,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2038</v>
       </c>
@@ -2567,7 +2594,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2039</v>
       </c>
@@ -2582,7 +2609,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2040</v>
       </c>
@@ -2596,7 +2623,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2041</v>
       </c>
@@ -2611,7 +2638,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2042</v>
       </c>
@@ -2626,7 +2653,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2043</v>
       </c>
@@ -2641,7 +2668,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2044</v>
       </c>
@@ -2656,7 +2683,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2045</v>
       </c>
@@ -2671,7 +2698,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2046</v>
       </c>
@@ -2686,7 +2713,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2047</v>
       </c>
@@ -2701,7 +2728,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2048</v>
       </c>
@@ -2716,7 +2743,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2049</v>
       </c>
@@ -2731,7 +2758,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2050</v>
       </c>
@@ -2763,17 +2790,17 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.625" customWidth="1"/>
-    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2793,7 +2820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -2813,7 +2840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -2829,7 +2856,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -2845,7 +2872,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -2861,7 +2888,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -2877,7 +2904,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2024</v>
       </c>
@@ -2893,7 +2920,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2025</v>
       </c>
@@ -2909,7 +2936,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2026</v>
       </c>
@@ -2925,7 +2952,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2027</v>
       </c>
@@ -2941,7 +2968,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2028</v>
       </c>
@@ -2957,7 +2984,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2029</v>
       </c>
@@ -2973,7 +3000,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2030</v>
       </c>
@@ -2989,7 +3016,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2031</v>
       </c>
@@ -3005,7 +3032,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2032</v>
       </c>
@@ -3021,7 +3048,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2033</v>
       </c>
@@ -3037,7 +3064,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2034</v>
       </c>
@@ -3053,7 +3080,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2035</v>
       </c>
@@ -3069,7 +3096,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2036</v>
       </c>
@@ -3085,7 +3112,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2037</v>
       </c>
@@ -3101,7 +3128,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2038</v>
       </c>
@@ -3117,7 +3144,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2039</v>
       </c>
@@ -3132,13 +3159,13 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2040</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>17159962249842.563</v>
+        <v>17159962249842.562</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -3147,7 +3174,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2041</v>
       </c>
@@ -3175,18 +3202,18 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69.5" customWidth="1"/>
-    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3206,12 +3233,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -3223,7 +3250,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -3233,7 +3260,7 @@
       <c r="C4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -3243,7 +3270,7 @@
       <c r="C5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -3253,7 +3280,7 @@
       <c r="C6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2024</v>
       </c>
@@ -3263,7 +3290,7 @@
       <c r="C7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2025</v>
       </c>
@@ -3275,7 +3302,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2026</v>
       </c>
@@ -3283,7 +3310,7 @@
         <v>10400000000000</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2027</v>
       </c>
@@ -3291,7 +3318,7 @@
         <v>10800000000000</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2028</v>
       </c>
@@ -3299,7 +3326,7 @@
         <v>11200000000000</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2029</v>
       </c>
@@ -3307,7 +3334,7 @@
         <v>11600000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2030</v>
       </c>
@@ -3315,7 +3342,7 @@
         <v>12000000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2031</v>
       </c>
@@ -3323,7 +3350,7 @@
         <v>12400000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2032</v>
       </c>
@@ -3331,7 +3358,7 @@
         <v>12800000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2033</v>
       </c>
@@ -3339,7 +3366,7 @@
         <v>13200000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2034</v>
       </c>
@@ -3347,7 +3374,7 @@
         <v>13600000000000</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2035</v>
       </c>
@@ -3355,7 +3382,7 @@
         <v>14000000000000</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2036</v>
       </c>
@@ -3363,7 +3390,7 @@
         <v>14400000000000</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2037</v>
       </c>
@@ -3371,7 +3398,7 @@
         <v>14800000000000</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2038</v>
       </c>
@@ -3379,7 +3406,7 @@
         <v>15200000000000</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2039</v>
       </c>
@@ -3387,7 +3414,7 @@
         <v>15600000000000</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2040</v>
       </c>
@@ -3398,7 +3425,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2041</v>
       </c>
@@ -3406,7 +3433,7 @@
         <v>16600000000000</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2042</v>
       </c>
@@ -3414,7 +3441,7 @@
         <v>17200000000000</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2043</v>
       </c>
@@ -3422,7 +3449,7 @@
         <v>17800000000000</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2044</v>
       </c>
@@ -3430,7 +3457,7 @@
         <v>18400000000000</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2045</v>
       </c>
@@ -3438,7 +3465,7 @@
         <v>19000000000000</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2046</v>
       </c>
@@ -3446,7 +3473,7 @@
         <v>19600000000000</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2047</v>
       </c>
@@ -3454,7 +3481,7 @@
         <v>20200000000000</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2048</v>
       </c>
@@ -3462,7 +3489,7 @@
         <v>20800000000000</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2049</v>
       </c>
@@ -3470,7 +3497,7 @@
         <v>21400000000000</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2050</v>
       </c>
@@ -3494,19 +3521,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EB8B21-702D-7B44-9AAA-37E8D9323EE6}">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="143" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B66"/>
+    <sheetView zoomScale="143" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.375" customWidth="1"/>
-    <col min="5" max="6" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
+    <col min="5" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
@@ -3514,7 +3541,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -3534,7 +3561,7 @@
         <v>6977931034482.7549</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -3551,7 +3578,7 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -3568,7 +3595,7 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -3585,7 +3612,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -3602,7 +3629,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -3619,7 +3646,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -3636,7 +3663,7 @@
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -3653,7 +3680,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -3670,7 +3697,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -3687,7 +3714,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -3707,7 +3734,7 @@
         <v>7291034482758.6182</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -3724,7 +3751,7 @@
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -3741,7 +3768,7 @@
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -3758,7 +3785,7 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -3775,7 +3802,7 @@
       </c>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -3792,7 +3819,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -3809,7 +3836,7 @@
       </c>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
@@ -3826,7 +3853,7 @@
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
@@ -3843,7 +3870,7 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>32</v>
       </c>
@@ -3860,7 +3887,7 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -3880,7 +3907,7 @@
         <v>3211034482750.5479</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>69</v>
       </c>
@@ -3897,7 +3924,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>78</v>
       </c>
@@ -3914,7 +3941,7 @@
       </c>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
@@ -3931,7 +3958,7 @@
       </c>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
@@ -3948,7 +3975,7 @@
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>79</v>
       </c>
@@ -3965,7 +3992,7 @@
       </c>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
@@ -3982,7 +4009,7 @@
       </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>70</v>
       </c>
@@ -3999,7 +4026,7 @@
       </c>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
@@ -4016,7 +4043,7 @@
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>38</v>
       </c>
@@ -4033,7 +4060,7 @@
       </c>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>39</v>
       </c>
@@ -4050,7 +4077,7 @@
       </c>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>71</v>
       </c>
@@ -4070,7 +4097,7 @@
         <v>2628275862068.9609</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>40</v>
       </c>
@@ -4087,7 +4114,7 @@
       </c>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
@@ -4104,7 +4131,7 @@
       </c>
       <c r="F35" s="7"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>42</v>
       </c>
@@ -4121,7 +4148,7 @@
       </c>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
@@ -4138,7 +4165,7 @@
       </c>
       <c r="F37" s="7"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>44</v>
       </c>
@@ -4155,7 +4182,7 @@
       </c>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>45</v>
       </c>
@@ -4172,7 +4199,7 @@
       </c>
       <c r="F39" s="7"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>72</v>
       </c>
@@ -4189,7 +4216,7 @@
       </c>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>46</v>
       </c>
@@ -4206,7 +4233,7 @@
       </c>
       <c r="F41" s="7"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>47</v>
       </c>
@@ -4226,7 +4253,7 @@
         <v>5799999999999.9961</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>73</v>
       </c>
@@ -4243,7 +4270,7 @@
       </c>
       <c r="F43" s="7"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
@@ -4260,7 +4287,7 @@
       </c>
       <c r="F44" s="7"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>49</v>
       </c>
@@ -4277,7 +4304,7 @@
       </c>
       <c r="F45" s="7"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>50</v>
       </c>
@@ -4294,7 +4321,7 @@
       </c>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>51</v>
       </c>
@@ -4311,7 +4338,7 @@
       </c>
       <c r="F47" s="7"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>52</v>
       </c>
@@ -4328,7 +4355,7 @@
       </c>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>53</v>
       </c>
@@ -4345,7 +4372,7 @@
       </c>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>54</v>
       </c>
@@ -4362,7 +4389,7 @@
       </c>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>55</v>
       </c>
@@ -4379,7 +4406,7 @@
       </c>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>74</v>
       </c>
@@ -4396,7 +4423,7 @@
       </c>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>56</v>
       </c>
@@ -4413,7 +4440,7 @@
       </c>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>57</v>
       </c>
@@ -4433,7 +4460,7 @@
         <v>8037241379310.3428</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>75</v>
       </c>
@@ -4450,7 +4477,7 @@
       </c>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>58</v>
       </c>
@@ -4467,7 +4494,7 @@
       </c>
       <c r="F56" s="7"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>59</v>
       </c>
@@ -4484,7 +4511,7 @@
       </c>
       <c r="F57" s="7"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>60</v>
       </c>
@@ -4501,7 +4528,7 @@
       </c>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>61</v>
       </c>
@@ -4518,7 +4545,7 @@
       </c>
       <c r="F59" s="7"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>62</v>
       </c>
@@ -4535,7 +4562,7 @@
       </c>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>63</v>
       </c>
@@ -4552,7 +4579,7 @@
       </c>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>64</v>
       </c>
@@ -4569,7 +4596,7 @@
       </c>
       <c r="F62" s="7"/>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>65</v>
       </c>
@@ -4586,7 +4613,7 @@
       </c>
       <c r="F63" s="7"/>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>66</v>
       </c>
@@ -4603,7 +4630,7 @@
       </c>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>67</v>
       </c>
@@ -4620,7 +4647,7 @@
       </c>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>68</v>
       </c>
@@ -4636,7 +4663,7 @@
         <v>698620689655.172</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
     </row>
   </sheetData>
@@ -4650,4 +4677,32 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C65568-9FA4-2140-ACCC-D7686B0F58EC}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>